<commit_message>
Created dataset with Kohaku, Sanke and Showa. Performed train-test-val split and load into pytorch dataset.
</commit_message>
<xml_diff>
--- a/bigger_dataset/data/tags_df_edited.xlsx
+++ b/bigger_dataset/data/tags_df_edited.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annahan/Documents/GitHub/learning-fuze/project_koi/bigger_dataset/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{30D933EE-2779-FA47-B044-BA8C37582802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{9E9EAAF5-B9E4-0149-8D6D-4E4DA3693609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3080" yWindow="2060" windowWidth="28040" windowHeight="17440" xr2:uid="{18037879-6B6B-9A46-9BC2-CFCB5EE6D52B}"/>
+    <workbookView xWindow="-34820" yWindow="2500" windowWidth="28040" windowHeight="17440" xr2:uid="{18037879-6B6B-9A46-9BC2-CFCB5EE6D52B}"/>
   </bookViews>
   <sheets>
     <sheet name="tags_df" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tags_df!$A$1:$F$159</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tags_df!$A$1:$G$159</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="185">
   <si>
     <t>tags</t>
   </si>
@@ -517,7 +517,67 @@
     <t>x</t>
   </si>
   <si>
-    <t>don't include</t>
+    <t>broad</t>
+  </si>
+  <si>
+    <t>goldfish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hariwake koi are a popular variety known for their shimmering, metallic platinum-white base and bold, vibrant patterns of red, yellow, or orange. They are a type of "Hikarimoyo" koi, meaning one color on a platinum background. </t>
+  </si>
+  <si>
+    <t>sub-variety</t>
+  </si>
+  <si>
+    <t>The Kujaku koi, also known as the “Peacock” koi, is a dazzling and unique variety of koi fish cherished for its intricate and vibrant pattern. Coming from Japan, this koi is a member of the Hikarimoyo class that is known for their metallic sheen and multicolored beauty.</t>
+  </si>
+  <si>
+    <t>This category includes all Koi with shiny bodies but devoid of any markings. Hikari Muji is divided into “Yamabuki Ogon” (with pure yellow, and a metallic sheen on the entire body), “Platinum Ogon” (with shining platinum color), “Orange Ogon” (with orange sheen), “Kin Matsuba” (literally “golden pine needles,” for individual, glittering scales appearing like raised markings), and “Gin Matsuba” (literally “silvery pine needles,” for glittering scales on the platinum ground which look like raised markings), etc.</t>
+  </si>
+  <si>
+    <t>MIXED??</t>
+  </si>
+  <si>
+    <t>Matsuba koi are a sub-variety of koi that are all single-coloured koi with a black net-like reticulation pattern, some Matsuba varieties, such as Gin Matsuba and Kin Matsuba, are metallic koi while other Matsuba varieties, such as Ki Matsuba and Shiro Matsuba are non-metallic koi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Utsurimono" and "Utsuri" are essentially the same thing in the context of koi fish. "Utsurimono" is the full Japanese name, while "Utsuri" is the shortened version. They both refer to a subvariety of koi with a dark base color (usually black) and contrasting patterns of another color. </t>
+  </si>
+  <si>
+    <t>A Kikusui is also often described as a metallic, Doitsu Kohaku koi as it is a scaleless, white koi with a red pattern over the white and a reflective sheen, or lustre, in the skin of the koi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ogon koi are a type of koi fish characterized by their single, metallic color, which can range from gold to silver. They are part of the Hikarimuji class, meaning "shiny, one". Ogon koi are known for their brilliant luster and graceful simplicity, making them a beautiful contrast to multi-colored varieties. </t>
+  </si>
+  <si>
+    <t>Kawarimono in Japanese means oddballs. So in Koi, Kawarimono basically includes most of the varieties that do not blog to the other groups.</t>
+  </si>
+  <si>
+    <t>sub-sub-variety</t>
+  </si>
+  <si>
+    <t>Kikokuryu koi fish (KEE-koh-KOO-droo) is a metallic, doitsu (or scaleless) koi with a white body overlaid with black scales in various patterns. It owes its pattern and coloration to the crossbreeding of Platinum Ogon and Kumonryu.</t>
+  </si>
+  <si>
+    <t>Kikokiryu</t>
+  </si>
+  <si>
+    <t>Yamato Nishiki are metallic Sanke. Yamato Nishiki come as both scaled and scaleless varieties. Scaleless skin (known as Doitsu) is derived from cross breeding Koi with similarly scaleless German mirror carp.</t>
+  </si>
+  <si>
+    <t>The Yamabuki is a solid, metallic yellow-colored koi and is part of a single-colored metallic koi class, the Hikarimuji (hee-KAH-ree-MOO-gee).</t>
+  </si>
+  <si>
+    <t>White colouration. Specifically refers to white as the base colour</t>
+  </si>
+  <si>
+    <t>a fairly new variety of Koi, created in the mid-90's by cross breeding Chagoi with Sorogoi. The result is a Koi with a Silver/Grey background or base skin colour, overlaid with striking patterns of Bronze/Gold.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goromo are a distinct variety of koi, often referred to as "robed koi". They are a cross between Kohaku and Asagi koi, resulting in a white body with red patterns similar to Kohaku, but with blue, black, or purple reticulation (netting) on the red scales. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heisei Nishiki is the name given to the doitsu (scaleless) version of Yamato Nishiki. </t>
   </si>
 </sst>
 </file>
@@ -660,7 +720,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -840,6 +900,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -1016,9 +1082,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1394,19 +1461,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AA76162-E944-A340-87E6-26245D433829}">
-  <dimension ref="A1:F159"/>
+  <dimension ref="A1:J159"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="151" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.1640625" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1417,16 +1488,25 @@
         <v>160</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>161</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>99</v>
       </c>
@@ -1439,8 +1519,11 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>97</v>
       </c>
@@ -1453,8 +1536,11 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>98</v>
       </c>
@@ -1467,8 +1553,11 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>100</v>
       </c>
@@ -1481,8 +1570,11 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>102</v>
       </c>
@@ -1492,9 +1584,14 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>103</v>
       </c>
@@ -1504,9 +1601,16 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>114</v>
       </c>
@@ -1514,13 +1618,16 @@
         <v>795</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -1530,9 +1637,21 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
@@ -1542,9 +1661,21 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>107</v>
       </c>
@@ -1553,12 +1684,15 @@
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>163</v>
+        <v>81</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>108</v>
       </c>
@@ -1567,12 +1701,15 @@
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>163</v>
+        <v>81</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>109</v>
       </c>
@@ -1581,12 +1718,15 @@
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>163</v>
+        <v>81</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>110</v>
       </c>
@@ -1599,8 +1739,11 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
@@ -1609,10 +1752,15 @@
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="E15" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>3</v>
       </c>
@@ -1621,10 +1769,15 @@
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="E16" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>101</v>
       </c>
@@ -1634,9 +1787,14 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F17" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
@@ -1646,9 +1804,16 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F18" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -1658,9 +1823,16 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F19" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>115</v>
       </c>
@@ -1670,9 +1842,19 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
@@ -1681,10 +1863,15 @@
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
+      <c r="E21" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>4</v>
       </c>
@@ -1694,10 +1881,17 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="F22" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>141</v>
       </c>
       <c r="B23" s="1">
@@ -1707,8 +1901,14 @@
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>12</v>
       </c>
@@ -1719,8 +1919,16 @@
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>64</v>
       </c>
@@ -1729,10 +1937,15 @@
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+      <c r="E25" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>14</v>
       </c>
@@ -1743,8 +1956,16 @@
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>128</v>
       </c>
@@ -1752,11 +1973,16 @@
         <v>103</v>
       </c>
       <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
+      <c r="D27" s="1" t="s">
+        <v>128</v>
+      </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>73</v>
       </c>
@@ -1765,10 +1991,24 @@
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
+      <c r="E28" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J28" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>67</v>
       </c>
@@ -1779,8 +2019,18 @@
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I29" s="1"/>
+      <c r="J29" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>33</v>
       </c>
@@ -1791,8 +2041,16 @@
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>46</v>
       </c>
@@ -1803,8 +2061,16 @@
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>116</v>
       </c>
@@ -1815,8 +2081,18 @@
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I32" s="1"/>
+      <c r="J32" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>71</v>
       </c>
@@ -1827,8 +2103,13 @@
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G33" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>118</v>
       </c>
@@ -1837,10 +2118,19 @@
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
+      <c r="E34" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="F34" s="1"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G34" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>19</v>
       </c>
@@ -1849,10 +2139,15 @@
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
+      <c r="E35" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="F35" s="1"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>42</v>
       </c>
@@ -1863,8 +2158,13 @@
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G36" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>15</v>
       </c>
@@ -1875,8 +2175,13 @@
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G37" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>44</v>
       </c>
@@ -1887,8 +2192,18 @@
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G38" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I38" s="1"/>
+      <c r="J38" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>13</v>
       </c>
@@ -1897,10 +2212,15 @@
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
+      <c r="E39" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="F39" s="1"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>18</v>
       </c>
@@ -1909,10 +2229,18 @@
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
+      <c r="E40" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="F40" s="1"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>96</v>
       </c>
@@ -1923,8 +2251,13 @@
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G41" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>111</v>
       </c>
@@ -1932,11 +2265,16 @@
         <v>48</v>
       </c>
       <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
+      <c r="D42" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>113</v>
       </c>
@@ -1944,11 +2282,16 @@
         <v>48</v>
       </c>
       <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
+      <c r="D43" s="1" t="s">
+        <v>113</v>
+      </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>9</v>
       </c>
@@ -1959,8 +2302,16 @@
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>41</v>
       </c>
@@ -1971,8 +2322,16 @@
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G45" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>122</v>
       </c>
@@ -1981,10 +2340,20 @@
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
+      <c r="E46" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="F46" s="1"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G46" s="1"/>
+      <c r="H46" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I46" s="1"/>
+      <c r="J46" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>125</v>
       </c>
@@ -1995,8 +2364,11 @@
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>30</v>
       </c>
@@ -2007,8 +2379,11 @@
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>10</v>
       </c>
@@ -2019,8 +2394,11 @@
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>119</v>
       </c>
@@ -2031,8 +2409,11 @@
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>17</v>
       </c>
@@ -2043,8 +2424,11 @@
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>63</v>
       </c>
@@ -2055,8 +2439,11 @@
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>138</v>
       </c>
@@ -2067,8 +2454,11 @@
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>121</v>
       </c>
@@ -2079,8 +2469,11 @@
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>62</v>
       </c>
@@ -2091,8 +2484,11 @@
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>31</v>
       </c>
@@ -2103,8 +2499,11 @@
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>104</v>
       </c>
@@ -2115,8 +2514,11 @@
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>127</v>
       </c>
@@ -2127,8 +2529,11 @@
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>20</v>
       </c>
@@ -2139,8 +2544,11 @@
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>117</v>
       </c>
@@ -2151,8 +2559,11 @@
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>11</v>
       </c>
@@ -2163,8 +2574,11 @@
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>106</v>
       </c>
@@ -2175,8 +2589,11 @@
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>123</v>
       </c>
@@ -2187,8 +2604,11 @@
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>124</v>
       </c>
@@ -2199,8 +2619,11 @@
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>105</v>
       </c>
@@ -2211,8 +2634,11 @@
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>32</v>
       </c>
@@ -2223,8 +2649,11 @@
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>68</v>
       </c>
@@ -2235,8 +2664,11 @@
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>38</v>
       </c>
@@ -2247,8 +2679,11 @@
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>133</v>
       </c>
@@ -2259,8 +2694,11 @@
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>147</v>
       </c>
@@ -2271,8 +2709,11 @@
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>43</v>
       </c>
@@ -2283,8 +2724,11 @@
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>80</v>
       </c>
@@ -2295,8 +2739,11 @@
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>137</v>
       </c>
@@ -2307,8 +2754,11 @@
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>90</v>
       </c>
@@ -2319,8 +2769,11 @@
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G74" s="1"/>
+      <c r="H74" s="1"/>
+      <c r="I74" s="1"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>6</v>
       </c>
@@ -2331,8 +2784,11 @@
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>120</v>
       </c>
@@ -2343,8 +2799,11 @@
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G76" s="1"/>
+      <c r="H76" s="1"/>
+      <c r="I76" s="1"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>145</v>
       </c>
@@ -2355,8 +2814,11 @@
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G77" s="1"/>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>21</v>
       </c>
@@ -2367,8 +2829,11 @@
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G78" s="1"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>47</v>
       </c>
@@ -2379,8 +2844,11 @@
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G79" s="1"/>
+      <c r="H79" s="1"/>
+      <c r="I79" s="1"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>77</v>
       </c>
@@ -2391,8 +2859,11 @@
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G80" s="1"/>
+      <c r="H80" s="1"/>
+      <c r="I80" s="1"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>78</v>
       </c>
@@ -2403,8 +2874,11 @@
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G81" s="1"/>
+      <c r="H81" s="1"/>
+      <c r="I81" s="1"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>112</v>
       </c>
@@ -2415,8 +2889,11 @@
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G82" s="1"/>
+      <c r="H82" s="1"/>
+      <c r="I82" s="1"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>155</v>
       </c>
@@ -2427,8 +2904,11 @@
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G83" s="1"/>
+      <c r="H83" s="1"/>
+      <c r="I83" s="1"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>81</v>
       </c>
@@ -2439,8 +2919,11 @@
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G84" s="1"/>
+      <c r="H84" s="1"/>
+      <c r="I84" s="1"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>131</v>
       </c>
@@ -2451,8 +2934,11 @@
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G85" s="1"/>
+      <c r="H85" s="1"/>
+      <c r="I85" s="1"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>159</v>
       </c>
@@ -2463,8 +2949,11 @@
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G86" s="1"/>
+      <c r="H86" s="1"/>
+      <c r="I86" s="1"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>52</v>
       </c>
@@ -2475,8 +2964,11 @@
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G87" s="1"/>
+      <c r="H87" s="1"/>
+      <c r="I87" s="1"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>74</v>
       </c>
@@ -2487,8 +2979,11 @@
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G88" s="1"/>
+      <c r="H88" s="1"/>
+      <c r="I88" s="1"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>146</v>
       </c>
@@ -2499,8 +2994,11 @@
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G89" s="1"/>
+      <c r="H89" s="1"/>
+      <c r="I89" s="1"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>151</v>
       </c>
@@ -2511,8 +3009,11 @@
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G90" s="1"/>
+      <c r="H90" s="1"/>
+      <c r="I90" s="1"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>126</v>
       </c>
@@ -2523,8 +3024,11 @@
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G91" s="1"/>
+      <c r="H91" s="1"/>
+      <c r="I91" s="1"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>129</v>
       </c>
@@ -2535,8 +3039,11 @@
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G92" s="1"/>
+      <c r="H92" s="1"/>
+      <c r="I92" s="1"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>8</v>
       </c>
@@ -2547,8 +3054,11 @@
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G93" s="1"/>
+      <c r="H93" s="1"/>
+      <c r="I93" s="1"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>35</v>
       </c>
@@ -2559,8 +3069,11 @@
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
       <c r="F94" s="1"/>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G94" s="1"/>
+      <c r="H94" s="1"/>
+      <c r="I94" s="1"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>66</v>
       </c>
@@ -2571,8 +3084,11 @@
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
       <c r="F95" s="1"/>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G95" s="1"/>
+      <c r="H95" s="1"/>
+      <c r="I95" s="1"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>135</v>
       </c>
@@ -2583,8 +3099,11 @@
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G96" s="1"/>
+      <c r="H96" s="1"/>
+      <c r="I96" s="1"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>140</v>
       </c>
@@ -2595,8 +3114,11 @@
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G97" s="1"/>
+      <c r="H97" s="1"/>
+      <c r="I97" s="1"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>144</v>
       </c>
@@ -2607,8 +3129,11 @@
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G98" s="1"/>
+      <c r="H98" s="1"/>
+      <c r="I98" s="1"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>152</v>
       </c>
@@ -2619,8 +3144,11 @@
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G99" s="1"/>
+      <c r="H99" s="1"/>
+      <c r="I99" s="1"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>132</v>
       </c>
@@ -2631,8 +3159,11 @@
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
       <c r="F100" s="1"/>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G100" s="1"/>
+      <c r="H100" s="1"/>
+      <c r="I100" s="1"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>26</v>
       </c>
@@ -2643,8 +3174,11 @@
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
       <c r="F101" s="1"/>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G101" s="1"/>
+      <c r="H101" s="1"/>
+      <c r="I101" s="1"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>142</v>
       </c>
@@ -2655,8 +3189,11 @@
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
       <c r="F102" s="1"/>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G102" s="1"/>
+      <c r="H102" s="1"/>
+      <c r="I102" s="1"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>143</v>
       </c>
@@ -2667,8 +3204,11 @@
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
       <c r="F103" s="1"/>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G103" s="1"/>
+      <c r="H103" s="1"/>
+      <c r="I103" s="1"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>34</v>
       </c>
@@ -2679,8 +3219,11 @@
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
       <c r="F104" s="1"/>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G104" s="1"/>
+      <c r="H104" s="1"/>
+      <c r="I104" s="1"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>40</v>
       </c>
@@ -2691,8 +3234,11 @@
       <c r="D105" s="1"/>
       <c r="E105" s="1"/>
       <c r="F105" s="1"/>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G105" s="1"/>
+      <c r="H105" s="1"/>
+      <c r="I105" s="1"/>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>70</v>
       </c>
@@ -2703,8 +3249,11 @@
       <c r="D106" s="1"/>
       <c r="E106" s="1"/>
       <c r="F106" s="1"/>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G106" s="1"/>
+      <c r="H106" s="1"/>
+      <c r="I106" s="1"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>136</v>
       </c>
@@ -2715,8 +3264,11 @@
       <c r="D107" s="1"/>
       <c r="E107" s="1"/>
       <c r="F107" s="1"/>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G107" s="1"/>
+      <c r="H107" s="1"/>
+      <c r="I107" s="1"/>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>148</v>
       </c>
@@ -2727,8 +3279,11 @@
       <c r="D108" s="1"/>
       <c r="E108" s="1"/>
       <c r="F108" s="1"/>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G108" s="1"/>
+      <c r="H108" s="1"/>
+      <c r="I108" s="1"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>23</v>
       </c>
@@ -2739,8 +3294,11 @@
       <c r="D109" s="1"/>
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G109" s="1"/>
+      <c r="H109" s="1"/>
+      <c r="I109" s="1"/>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>24</v>
       </c>
@@ -2751,8 +3309,11 @@
       <c r="D110" s="1"/>
       <c r="E110" s="1"/>
       <c r="F110" s="1"/>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G110" s="1"/>
+      <c r="H110" s="1"/>
+      <c r="I110" s="1"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>29</v>
       </c>
@@ -2763,8 +3324,11 @@
       <c r="D111" s="1"/>
       <c r="E111" s="1"/>
       <c r="F111" s="1"/>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G111" s="1"/>
+      <c r="H111" s="1"/>
+      <c r="I111" s="1"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>48</v>
       </c>
@@ -2775,8 +3339,11 @@
       <c r="D112" s="1"/>
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G112" s="1"/>
+      <c r="H112" s="1"/>
+      <c r="I112" s="1"/>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>53</v>
       </c>
@@ -2787,8 +3354,11 @@
       <c r="D113" s="1"/>
       <c r="E113" s="1"/>
       <c r="F113" s="1"/>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G113" s="1"/>
+      <c r="H113" s="1"/>
+      <c r="I113" s="1"/>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>54</v>
       </c>
@@ -2799,8 +3369,11 @@
       <c r="D114" s="1"/>
       <c r="E114" s="1"/>
       <c r="F114" s="1"/>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G114" s="1"/>
+      <c r="H114" s="1"/>
+      <c r="I114" s="1"/>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>69</v>
       </c>
@@ -2811,8 +3384,11 @@
       <c r="D115" s="1"/>
       <c r="E115" s="1"/>
       <c r="F115" s="1"/>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G115" s="1"/>
+      <c r="H115" s="1"/>
+      <c r="I115" s="1"/>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>82</v>
       </c>
@@ -2823,8 +3399,11 @@
       <c r="D116" s="1"/>
       <c r="E116" s="1"/>
       <c r="F116" s="1"/>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G116" s="1"/>
+      <c r="H116" s="1"/>
+      <c r="I116" s="1"/>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>83</v>
       </c>
@@ -2835,8 +3414,11 @@
       <c r="D117" s="1"/>
       <c r="E117" s="1"/>
       <c r="F117" s="1"/>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G117" s="1"/>
+      <c r="H117" s="1"/>
+      <c r="I117" s="1"/>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>89</v>
       </c>
@@ -2847,8 +3429,11 @@
       <c r="D118" s="1"/>
       <c r="E118" s="1"/>
       <c r="F118" s="1"/>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G118" s="1"/>
+      <c r="H118" s="1"/>
+      <c r="I118" s="1"/>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>95</v>
       </c>
@@ -2859,8 +3444,11 @@
       <c r="D119" s="1"/>
       <c r="E119" s="1"/>
       <c r="F119" s="1"/>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G119" s="1"/>
+      <c r="H119" s="1"/>
+      <c r="I119" s="1"/>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>139</v>
       </c>
@@ -2871,8 +3459,11 @@
       <c r="D120" s="1"/>
       <c r="E120" s="1"/>
       <c r="F120" s="1"/>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G120" s="1"/>
+      <c r="H120" s="1"/>
+      <c r="I120" s="1"/>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>149</v>
       </c>
@@ -2883,8 +3474,11 @@
       <c r="D121" s="1"/>
       <c r="E121" s="1"/>
       <c r="F121" s="1"/>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G121" s="1"/>
+      <c r="H121" s="1"/>
+      <c r="I121" s="1"/>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>150</v>
       </c>
@@ -2895,8 +3489,11 @@
       <c r="D122" s="1"/>
       <c r="E122" s="1"/>
       <c r="F122" s="1"/>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G122" s="1"/>
+      <c r="H122" s="1"/>
+      <c r="I122" s="1"/>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>153</v>
       </c>
@@ -2907,8 +3504,11 @@
       <c r="D123" s="1"/>
       <c r="E123" s="1"/>
       <c r="F123" s="1"/>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G123" s="1"/>
+      <c r="H123" s="1"/>
+      <c r="I123" s="1"/>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>154</v>
       </c>
@@ -2919,8 +3519,11 @@
       <c r="D124" s="1"/>
       <c r="E124" s="1"/>
       <c r="F124" s="1"/>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G124" s="1"/>
+      <c r="H124" s="1"/>
+      <c r="I124" s="1"/>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>158</v>
       </c>
@@ -2931,8 +3534,11 @@
       <c r="D125" s="1"/>
       <c r="E125" s="1"/>
       <c r="F125" s="1"/>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G125" s="1"/>
+      <c r="H125" s="1"/>
+      <c r="I125" s="1"/>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>5</v>
       </c>
@@ -2943,8 +3549,11 @@
       <c r="D126" s="1"/>
       <c r="E126" s="1"/>
       <c r="F126" s="1"/>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G126" s="1"/>
+      <c r="H126" s="1"/>
+      <c r="I126" s="1"/>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>25</v>
       </c>
@@ -2955,8 +3564,11 @@
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
       <c r="F127" s="1"/>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G127" s="1"/>
+      <c r="H127" s="1"/>
+      <c r="I127" s="1"/>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>36</v>
       </c>
@@ -2967,8 +3579,11 @@
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>
       <c r="F128" s="1"/>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G128" s="1"/>
+      <c r="H128" s="1"/>
+      <c r="I128" s="1"/>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>37</v>
       </c>
@@ -2979,8 +3594,11 @@
       <c r="D129" s="1"/>
       <c r="E129" s="1"/>
       <c r="F129" s="1"/>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G129" s="1"/>
+      <c r="H129" s="1"/>
+      <c r="I129" s="1"/>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>39</v>
       </c>
@@ -2991,8 +3609,11 @@
       <c r="D130" s="1"/>
       <c r="E130" s="1"/>
       <c r="F130" s="1"/>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G130" s="1"/>
+      <c r="H130" s="1"/>
+      <c r="I130" s="1"/>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>45</v>
       </c>
@@ -3003,8 +3624,11 @@
       <c r="D131" s="1"/>
       <c r="E131" s="1"/>
       <c r="F131" s="1"/>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G131" s="1"/>
+      <c r="H131" s="1"/>
+      <c r="I131" s="1"/>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>49</v>
       </c>
@@ -3015,8 +3639,11 @@
       <c r="D132" s="1"/>
       <c r="E132" s="1"/>
       <c r="F132" s="1"/>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G132" s="1"/>
+      <c r="H132" s="1"/>
+      <c r="I132" s="1"/>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>50</v>
       </c>
@@ -3027,8 +3654,11 @@
       <c r="D133" s="1"/>
       <c r="E133" s="1"/>
       <c r="F133" s="1"/>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G133" s="1"/>
+      <c r="H133" s="1"/>
+      <c r="I133" s="1"/>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>51</v>
       </c>
@@ -3039,8 +3669,11 @@
       <c r="D134" s="1"/>
       <c r="E134" s="1"/>
       <c r="F134" s="1"/>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G134" s="1"/>
+      <c r="H134" s="1"/>
+      <c r="I134" s="1"/>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>55</v>
       </c>
@@ -3051,8 +3684,11 @@
       <c r="D135" s="1"/>
       <c r="E135" s="1"/>
       <c r="F135" s="1"/>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G135" s="1"/>
+      <c r="H135" s="1"/>
+      <c r="I135" s="1"/>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>56</v>
       </c>
@@ -3063,8 +3699,11 @@
       <c r="D136" s="1"/>
       <c r="E136" s="1"/>
       <c r="F136" s="1"/>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G136" s="1"/>
+      <c r="H136" s="1"/>
+      <c r="I136" s="1"/>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>57</v>
       </c>
@@ -3075,8 +3714,11 @@
       <c r="D137" s="1"/>
       <c r="E137" s="1"/>
       <c r="F137" s="1"/>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G137" s="1"/>
+      <c r="H137" s="1"/>
+      <c r="I137" s="1"/>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>58</v>
       </c>
@@ -3087,8 +3729,11 @@
       <c r="D138" s="1"/>
       <c r="E138" s="1"/>
       <c r="F138" s="1"/>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G138" s="1"/>
+      <c r="H138" s="1"/>
+      <c r="I138" s="1"/>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>59</v>
       </c>
@@ -3099,8 +3744,11 @@
       <c r="D139" s="1"/>
       <c r="E139" s="1"/>
       <c r="F139" s="1"/>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G139" s="1"/>
+      <c r="H139" s="1"/>
+      <c r="I139" s="1"/>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>60</v>
       </c>
@@ -3111,8 +3759,11 @@
       <c r="D140" s="1"/>
       <c r="E140" s="1"/>
       <c r="F140" s="1"/>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G140" s="1"/>
+      <c r="H140" s="1"/>
+      <c r="I140" s="1"/>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>61</v>
       </c>
@@ -3123,8 +3774,11 @@
       <c r="D141" s="1"/>
       <c r="E141" s="1"/>
       <c r="F141" s="1"/>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G141" s="1"/>
+      <c r="H141" s="1"/>
+      <c r="I141" s="1"/>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>65</v>
       </c>
@@ -3135,8 +3789,11 @@
       <c r="D142" s="1"/>
       <c r="E142" s="1"/>
       <c r="F142" s="1"/>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G142" s="1"/>
+      <c r="H142" s="1"/>
+      <c r="I142" s="1"/>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>72</v>
       </c>
@@ -3147,8 +3804,11 @@
       <c r="D143" s="1"/>
       <c r="E143" s="1"/>
       <c r="F143" s="1"/>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G143" s="1"/>
+      <c r="H143" s="1"/>
+      <c r="I143" s="1"/>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>75</v>
       </c>
@@ -3159,8 +3819,11 @@
       <c r="D144" s="1"/>
       <c r="E144" s="1"/>
       <c r="F144" s="1"/>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G144" s="1"/>
+      <c r="H144" s="1"/>
+      <c r="I144" s="1"/>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>76</v>
       </c>
@@ -3171,8 +3834,11 @@
       <c r="D145" s="1"/>
       <c r="E145" s="1"/>
       <c r="F145" s="1"/>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G145" s="1"/>
+      <c r="H145" s="1"/>
+      <c r="I145" s="1"/>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>79</v>
       </c>
@@ -3183,8 +3849,11 @@
       <c r="D146" s="1"/>
       <c r="E146" s="1"/>
       <c r="F146" s="1"/>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G146" s="1"/>
+      <c r="H146" s="1"/>
+      <c r="I146" s="1"/>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>84</v>
       </c>
@@ -3195,8 +3864,11 @@
       <c r="D147" s="1"/>
       <c r="E147" s="1"/>
       <c r="F147" s="1"/>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G147" s="1"/>
+      <c r="H147" s="1"/>
+      <c r="I147" s="1"/>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>85</v>
       </c>
@@ -3207,8 +3879,11 @@
       <c r="D148" s="1"/>
       <c r="E148" s="1"/>
       <c r="F148" s="1"/>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G148" s="1"/>
+      <c r="H148" s="1"/>
+      <c r="I148" s="1"/>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>86</v>
       </c>
@@ -3219,8 +3894,11 @@
       <c r="D149" s="1"/>
       <c r="E149" s="1"/>
       <c r="F149" s="1"/>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G149" s="1"/>
+      <c r="H149" s="1"/>
+      <c r="I149" s="1"/>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>87</v>
       </c>
@@ -3231,8 +3909,11 @@
       <c r="D150" s="1"/>
       <c r="E150" s="1"/>
       <c r="F150" s="1"/>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G150" s="1"/>
+      <c r="H150" s="1"/>
+      <c r="I150" s="1"/>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>88</v>
       </c>
@@ -3243,8 +3924,11 @@
       <c r="D151" s="1"/>
       <c r="E151" s="1"/>
       <c r="F151" s="1"/>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G151" s="1"/>
+      <c r="H151" s="1"/>
+      <c r="I151" s="1"/>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>91</v>
       </c>
@@ -3255,8 +3939,11 @@
       <c r="D152" s="1"/>
       <c r="E152" s="1"/>
       <c r="F152" s="1"/>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G152" s="1"/>
+      <c r="H152" s="1"/>
+      <c r="I152" s="1"/>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>92</v>
       </c>
@@ -3267,8 +3954,11 @@
       <c r="D153" s="1"/>
       <c r="E153" s="1"/>
       <c r="F153" s="1"/>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G153" s="1"/>
+      <c r="H153" s="1"/>
+      <c r="I153" s="1"/>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>93</v>
       </c>
@@ -3279,8 +3969,11 @@
       <c r="D154" s="1"/>
       <c r="E154" s="1"/>
       <c r="F154" s="1"/>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G154" s="1"/>
+      <c r="H154" s="1"/>
+      <c r="I154" s="1"/>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>94</v>
       </c>
@@ -3291,8 +3984,11 @@
       <c r="D155" s="1"/>
       <c r="E155" s="1"/>
       <c r="F155" s="1"/>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G155" s="1"/>
+      <c r="H155" s="1"/>
+      <c r="I155" s="1"/>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>130</v>
       </c>
@@ -3303,8 +3999,11 @@
       <c r="D156" s="1"/>
       <c r="E156" s="1"/>
       <c r="F156" s="1"/>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G156" s="1"/>
+      <c r="H156" s="1"/>
+      <c r="I156" s="1"/>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>134</v>
       </c>
@@ -3315,8 +4014,11 @@
       <c r="D157" s="1"/>
       <c r="E157" s="1"/>
       <c r="F157" s="1"/>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G157" s="1"/>
+      <c r="H157" s="1"/>
+      <c r="I157" s="1"/>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>156</v>
       </c>
@@ -3327,8 +4029,11 @@
       <c r="D158" s="1"/>
       <c r="E158" s="1"/>
       <c r="F158" s="1"/>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G158" s="1"/>
+      <c r="H158" s="1"/>
+      <c r="I158" s="1"/>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>157</v>
       </c>
@@ -3339,9 +4044,12 @@
       <c r="D159" s="1"/>
       <c r="E159" s="1"/>
       <c r="F159" s="1"/>
+      <c r="G159" s="1"/>
+      <c r="H159" s="1"/>
+      <c r="I159" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F159" xr:uid="{2AA76162-E944-A340-87E6-26245D433829}"/>
+  <autoFilter ref="A1:G159" xr:uid="{2AA76162-E944-A340-87E6-26245D433829}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Calculated gradcam on incorrect predictions.
</commit_message>
<xml_diff>
--- a/bigger_dataset/data/tags_df_edited.xlsx
+++ b/bigger_dataset/data/tags_df_edited.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annahan/Documents/GitHub/learning-fuze/project_koi/bigger_dataset/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{9E9EAAF5-B9E4-0149-8D6D-4E4DA3693609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F589A8E7-0ACA-5C42-8EBD-EC6DDE83DFC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34820" yWindow="2500" windowWidth="28040" windowHeight="17440" xr2:uid="{18037879-6B6B-9A46-9BC2-CFCB5EE6D52B}"/>
+    <workbookView xWindow="37740" yWindow="540" windowWidth="28040" windowHeight="17440" xr2:uid="{18037879-6B6B-9A46-9BC2-CFCB5EE6D52B}"/>
   </bookViews>
   <sheets>
     <sheet name="tags_df" sheetId="1" r:id="rId1"/>
@@ -1464,8 +1464,8 @@
   <dimension ref="A1:J159"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E47" sqref="E47"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1778,7 +1778,7 @@
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="2" t="s">
         <v>101</v>
       </c>
       <c r="B17" s="1">
@@ -1795,7 +1795,7 @@
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B18" s="1">
@@ -1814,7 +1814,7 @@
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="1">

</xml_diff>